<commit_message>
Convert from rems to bems
</commit_message>
<xml_diff>
--- a/REMS/wwwroot/reports/تقرير قسم المتابعة_20251028.xlsx
+++ b/REMS/wwwroot/reports/تقرير قسم المتابعة_20251028.xlsx
@@ -37,6 +37,45 @@
     <x:t>Path</x:t>
   </x:si>
   <x:si>
+    <x:t>Region</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Governorate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coordinator</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WorkDate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>StoreName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>StoreType</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ContractFilePath</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ContractFileName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ContractDate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AllTasksDone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ProductsCount</x:t>
+  </x:si>
+  <x:si>
     <x:t>CustomFieldsJson</x:t>
   </x:si>
   <x:si>
@@ -64,9 +103,6 @@
     <x:t>رقم الهاتف</x:t>
   </x:si>
   <x:si>
-    <x:t>توقيع العقد</x:t>
-  </x:si>
-  <x:si>
     <x:t>تاريخ العقد</x:t>
   </x:si>
   <x:si>
@@ -76,25 +112,127 @@
     <x:t>عدد المنتجات التي تم إدخالها</x:t>
   </x:si>
   <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>meriana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-10-28 17:03</x:t>
+    <x:t>توقيع العقد (ملف)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdsd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Admin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 17:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>نعم</x:t>
+  </x:si>
+  <x:si>
+    <x:t>منتهية</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdgdsg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdfgsdfg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dfgdfs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdgsd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>بقالة</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdgsdg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdgdg</x:t>
   </x:si>
   <x:si>
     <x:t>لا</x:t>
   </x:si>
   <x:si>
+    <x:t>[{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0637\u0642\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;sdgdsg&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062D\u0627\u0641\u0638\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;sdfgsdfg&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0633\u0642&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;dfgdfs&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0645\u0644&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;sdgsd&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0646\u0648\u0639 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0628\u0642\u0627\u0644\u0629&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0644\u0639\u0646\u0648\u0627\u0646&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;sdgsdg&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0631\u0642\u0645 \u0627\u0644\u0647\u0627\u062A\u0641&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;sdgdg&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0625\u0646\u062C\u0627\u0632 \u0643\u0627\u0641\u0629 \u0627\u0644\u0645\u0647\u0627\u0645&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;false&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0639\u062F\u062F \u0627\u0644\u0645\u0646\u062A\u062C\u0627\u062A \u0627\u0644\u062A\u064A \u062A\u0645 \u0625\u062F\u062E\u0627\u0644\u0647\u0627&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0648\u0642\u064A\u0639 \u0627\u0644\u0639\u0642\u062F (\u0645\u0644\u0641)&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;}]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>false</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sdvdsv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 17:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/Files/2025-10-28_17-26-56_d217d525-5e4e-44a3-8445-4b9e0f2b9771.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>damas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>haidra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dasda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>مخابز</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0958968338</x:t>
+  </x:si>
+  <x:si>
+    <x:t>images.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0637\u0642\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;damas&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062D\u0627\u0641\u0638\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;damas&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0633\u0642&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;haidra&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0645\u0644&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;dasda&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0646\u0648\u0639 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u062E\u0627\u0628\u0632&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0644\u0639\u0646\u0648\u0627\u0646&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;damas&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0631\u0642\u0645 \u0627\u0644\u0647\u0627\u062A\u0641&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;0958968338&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0625\u0646\u062C\u0627\u0632 \u0643\u0627\u0641\u0629 \u0627\u0644\u0645\u0647\u0627\u0645&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;true&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0639\u062F\u062F \u0627\u0644\u0645\u0646\u062A\u062C\u0627\u062A \u0627\u0644\u062A\u064A \u062A\u0645 \u0625\u062F\u062E\u0627\u0644\u0647\u0627&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;234&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0648\u0642\u064A\u0639 \u0627\u0644\u0639\u0642\u062F (\u0645\u0644\u0641)&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;/Files/2025-10-28_17-26-56_d217d525-5e4e-44a3-8445-4b9e0f2b9771.png&amp;quot;}]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>true</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 17:39</x:t>
+  </x:si>
+  <x:si>
     <x:t>غير منتهية</x:t>
   </x:si>
   <x:si>
-    <x:t>/Files/2025-10-28_17-03-43_28e6c10f-b12b-42fb-81cf-e501103c123c.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0637\u0642\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u0647\u0627\u062C\u0631\u064A\u0646&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062D\u0627\u0641\u0638\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u062F\u0645\u0634\u0642&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0633\u0642&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u062D\u064A\u062F\u0631\u0647 \u0627\u0628\u0648 \u062D\u0645\u0631\u0647&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0645\u0644&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Date&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0641\u0644\u0627\u0646 \u0627\u0644\u0641\u0644\u0627\u0646\u064A&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0646\u0648\u0639 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u0637\u0639\u0645&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0644\u0639\u0646\u0648\u0627\u0646&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u0647\u0627\u062C\u0631\u064A\u0646 \u0645\u0648\u0642\u0641 \u0627\u0644\u0628\u0627\u0634\u0643\u0627\u062A\u0628&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0631\u0642\u0645 \u0627\u0644\u0647\u0627\u062A\u0641&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Text&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;0958968338&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0648\u0642\u064A\u0639 \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;File&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;/Files/2025-10-28_17-03-43_28e6c10f-b12b-42fb-81cf-e501103c123c.pdf&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Date&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0625\u0646\u062C\u0627\u0632 \u0643\u0627\u0641\u0629 \u0627\u0644\u0645\u0647\u0627\u0645&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Checkbox&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;true&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0639\u062F\u062F \u0627\u0644\u0645\u0646\u062A\u062C\u0627\u062A \u0627\u0644\u062A\u064A \u062A\u0645 \u0625\u062F\u062E\u0627\u0644\u0647\u0627&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Number&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;5&amp;quot;}]</x:t>
+    <x:t>[{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0637\u0642\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062D\u0627\u0641\u0638\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0633\u0642&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0645\u0644&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0646\u0648\u0639 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0644\u0639\u0646\u0648\u0627\u0646&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0631\u0642\u0645 \u0627\u0644\u0647\u0627\u062A\u0641&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0625\u0646\u062C\u0627\u0632 \u0643\u0627\u0641\u0629 \u0627\u0644\u0645\u0647\u0627\u0645&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;false&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0639\u062F\u062F \u0627\u0644\u0645\u0646\u062A\u062C\u0627\u062A \u0627\u0644\u062A\u064A \u062A\u0645 \u0625\u062F\u062E\u0627\u0644\u0647\u0627&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0648\u0642\u064A\u0639 \u0627\u0644\u0639\u0642\u062F (\u0645\u0644\u0641)&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;}]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 17:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>جورج الدهيم</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-28 18:14</x:t>
   </x:si>
   <x:si>
     <x:t>مهاجرين</x:t>
@@ -103,28 +241,16 @@
     <x:t>دمشق</x:t>
   </x:si>
   <x:si>
-    <x:t>حيدره ابو حمره</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-10-28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>فلان الفلاني</x:t>
-  </x:si>
-  <x:si>
-    <x:t>مطعم</x:t>
-  </x:si>
-  <x:si>
-    <x:t>مهاجرين موقف الباشكاتب</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0958968338</x:t>
-  </x:si>
-  <x:si>
-    <x:t>true</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
+    <x:t>كوسا محشي</x:t>
+  </x:si>
+  <x:si>
+    <x:t>مهاجرين شارع ناظم باشا</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0637\u0642\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u0647\u0627\u062C\u0631\u064A\u0646&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062D\u0627\u0641\u0638\u0629&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u062F\u0645\u0634\u0642&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u0646\u0633\u0642&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0645\u0644&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0633\u0645 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0643\u0648\u0633\u0627 \u0645\u062D\u0634\u064A&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0646\u0648\u0639 \u0627\u0644\u0645\u062A\u062C\u0631&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0627\u0644\u0639\u0646\u0648\u0627\u0646&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;\u0645\u0647\u0627\u062C\u0631\u064A\u0646 \u0634\u0627\u0631\u0639 \u0646\u0627\u0638\u0645 \u0628\u0627\u0634\u0627&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0631\u0642\u0645 \u0627\u0644\u0647\u0627\u062A\u0641&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;0958968338&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0627\u0631\u064A\u062E \u0627\u0644\u0639\u0642\u062F&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;2025-10-28&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0625\u0646\u062C\u0627\u0632 \u0643\u0627\u0641\u0629 \u0627\u0644\u0645\u0647\u0627\u0645&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;false&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u0639\u062F\u062F \u0627\u0644\u0645\u0646\u062A\u062C\u0627\u062A \u0627\u0644\u062A\u064A \u062A\u0645 \u0625\u062F\u062E\u0627\u0644\u0647\u0627&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;15&amp;quot;},{&amp;quot;Name&amp;quot;:&amp;quot;\u062A\u0648\u0642\u064A\u0639 \u0627\u0644\u0639\u0642\u062F (\u0645\u0644\u0641)&amp;quot;,&amp;quot;Type&amp;quot;:&amp;quot;Basic&amp;quot;,&amp;quot;Value&amp;quot;:&amp;quot;&amp;quot;}]</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -500,7 +626,7 @@
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:T2"/>
+  <x:dimension ref="A1:AG6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -508,27 +634,40 @@
   <x:cols>
     <x:col min="1" max="1" width="2.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="8.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.282054" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.996339" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="15.710625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="7.282054" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="12.853482" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="64.424911" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="255" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="11.996339" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="13.282054" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="15.424911" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="12.567768" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="13.853482" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="11.282054" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="25.853482" style="0" customWidth="1"/>
-    <x:col min="16" max="16" width="11.424911" style="0" customWidth="1"/>
-    <x:col min="17" max="17" width="64.424911" style="0" customWidth="1"/>
-    <x:col min="18" max="18" width="12.710625" style="0" customWidth="1"/>
-    <x:col min="19" max="19" width="15.853482" style="0" customWidth="1"/>
-    <x:col min="20" max="20" width="28.996339" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="66.424911" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="8.567768" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="11.710625" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="15.710625" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="11.710625" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="9.996339" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="23.567768" style="0" customWidth="1"/>
+    <x:col min="15" max="15" width="11.282054" style="0" customWidth="1"/>
+    <x:col min="16" max="16" width="66.424911" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="16.853482" style="0" customWidth="1"/>
+    <x:col min="18" max="18" width="15.710625" style="0" customWidth="1"/>
+    <x:col min="19" max="19" width="12.853482" style="0" customWidth="1"/>
+    <x:col min="20" max="20" width="14.567768" style="0" customWidth="1"/>
+    <x:col min="21" max="21" width="255" style="0" customWidth="1"/>
+    <x:col min="22" max="22" width="11.996339" style="0" customWidth="1"/>
+    <x:col min="23" max="23" width="13.282054" style="0" customWidth="1"/>
+    <x:col min="24" max="24" width="11.567768" style="0" customWidth="1"/>
+    <x:col min="25" max="25" width="12.567768" style="0" customWidth="1"/>
+    <x:col min="26" max="26" width="11.710625" style="0" customWidth="1"/>
+    <x:col min="27" max="27" width="11.282054" style="0" customWidth="1"/>
+    <x:col min="28" max="28" width="23.567768" style="0" customWidth="1"/>
+    <x:col min="29" max="29" width="11.424911" style="0" customWidth="1"/>
+    <x:col min="30" max="30" width="12.710625" style="0" customWidth="1"/>
+    <x:col min="31" max="31" width="15.853482" style="0" customWidth="1"/>
+    <x:col min="32" max="32" width="28.996339" style="0" customWidth="1"/>
+    <x:col min="33" max="33" width="66.424911" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:20">
+    <x:row r="1" spans="1:33">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -589,66 +728,420 @@
       <x:c r="T1" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="U1" s="1" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="V1" s="1" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="W1" s="1" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="X1" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="Y1" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="Z1" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="AA1" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="AB1" s="1" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="AC1" s="1" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="AD1" s="1" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="AE1" s="1" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="AF1" s="1" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="AG1" s="1" t="s">
+        <x:v>32</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:20">
+    <x:row r="2" spans="1:33">
       <x:c r="A2" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s"/>
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
       <x:c r="C2" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E2" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F2" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G2" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="G2" s="1" t="s"/>
       <x:c r="H2" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="I2" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="J2" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="K2" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="L2" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="M2" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="N2" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="O2" s="1" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="P2" s="1" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="Q2" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="P2" s="1" t="s"/>
+      <x:c r="Q2" s="1" t="s"/>
       <x:c r="R2" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="S2" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="T2" s="1" t="s"/>
+      <x:c r="U2" s="1" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="V2" s="1" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="W2" s="1" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="X2" s="1" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="Y2" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Z2" s="1" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AA2" s="1" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="AB2" s="1" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AC2" s="1" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AD2" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE2" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AF2" s="1" t="s"/>
+      <x:c r="AG2" s="1" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:33">
+      <x:c r="A3" s="1" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="T2" s="1" t="s">
-        <x:v>36</x:v>
-      </x:c>
+      <x:c r="D3" s="1" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F3" s="1" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="G3" s="1" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="I3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="J3" s="1" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="K3" s="1" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="L3" s="1" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="M3" s="1" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="N3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="O3" s="1" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="P3" s="1" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Q3" s="1" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="R3" s="1" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="S3" s="1" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="T3" s="1" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="U3" s="1" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="V3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="W3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="X3" s="1" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Y3" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Z3" s="1" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AA3" s="1" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AB3" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="AC3" s="1" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AD3" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE3" s="1" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="AF3" s="1" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AG3" s="1" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:33">
+      <x:c r="A4" s="1" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s"/>
+      <x:c r="C4" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D4" s="1" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E4" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="F4" s="1" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="G4" s="1" t="s"/>
+      <x:c r="H4" s="1" t="s"/>
+      <x:c r="I4" s="1" t="s"/>
+      <x:c r="J4" s="1" t="s"/>
+      <x:c r="K4" s="1" t="s"/>
+      <x:c r="L4" s="1" t="s"/>
+      <x:c r="M4" s="1" t="s"/>
+      <x:c r="N4" s="1" t="s"/>
+      <x:c r="O4" s="1" t="s"/>
+      <x:c r="P4" s="1" t="s"/>
+      <x:c r="Q4" s="1" t="s"/>
+      <x:c r="R4" s="1" t="s"/>
+      <x:c r="S4" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="T4" s="1" t="s"/>
+      <x:c r="U4" s="1" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="V4" s="1" t="s"/>
+      <x:c r="W4" s="1" t="s"/>
+      <x:c r="X4" s="1" t="s"/>
+      <x:c r="Y4" s="1" t="s"/>
+      <x:c r="Z4" s="1" t="s"/>
+      <x:c r="AA4" s="1" t="s"/>
+      <x:c r="AB4" s="1" t="s"/>
+      <x:c r="AC4" s="1" t="s"/>
+      <x:c r="AD4" s="1" t="s"/>
+      <x:c r="AE4" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AF4" s="1" t="s"/>
+      <x:c r="AG4" s="1" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:33">
+      <x:c r="A5" s="1" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s"/>
+      <x:c r="C5" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="E5" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="F5" s="1" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="G5" s="1" t="s"/>
+      <x:c r="H5" s="1" t="s"/>
+      <x:c r="I5" s="1" t="s"/>
+      <x:c r="J5" s="1" t="s"/>
+      <x:c r="K5" s="1" t="s"/>
+      <x:c r="L5" s="1" t="s"/>
+      <x:c r="M5" s="1" t="s"/>
+      <x:c r="N5" s="1" t="s"/>
+      <x:c r="O5" s="1" t="s"/>
+      <x:c r="P5" s="1" t="s"/>
+      <x:c r="Q5" s="1" t="s"/>
+      <x:c r="R5" s="1" t="s"/>
+      <x:c r="S5" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="T5" s="1" t="s"/>
+      <x:c r="U5" s="1" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="V5" s="1" t="s"/>
+      <x:c r="W5" s="1" t="s"/>
+      <x:c r="X5" s="1" t="s"/>
+      <x:c r="Y5" s="1" t="s"/>
+      <x:c r="Z5" s="1" t="s"/>
+      <x:c r="AA5" s="1" t="s"/>
+      <x:c r="AB5" s="1" t="s"/>
+      <x:c r="AC5" s="1" t="s"/>
+      <x:c r="AD5" s="1" t="s"/>
+      <x:c r="AE5" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AF5" s="1" t="s"/>
+      <x:c r="AG5" s="1" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:33">
+      <x:c r="A6" s="1" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s"/>
+      <x:c r="C6" s="1" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="D6" s="1" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E6" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="F6" s="1" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="G6" s="1" t="s"/>
+      <x:c r="H6" s="1" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="I6" s="1" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="J6" s="1" t="s"/>
+      <x:c r="K6" s="1" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="L6" s="1" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="M6" s="1" t="s"/>
+      <x:c r="N6" s="1" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="O6" s="1" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="P6" s="1" t="s"/>
+      <x:c r="Q6" s="1" t="s"/>
+      <x:c r="R6" s="1" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="S6" s="1" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="T6" s="1" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="U6" s="1" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="V6" s="1" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="W6" s="1" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="X6" s="1" t="s"/>
+      <x:c r="Y6" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Z6" s="1" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="AA6" s="1" t="s"/>
+      <x:c r="AB6" s="1" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="AC6" s="1" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AD6" s="1" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE6" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AF6" s="1" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="AG6" s="1" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>